<commit_message>
[Design] WIP Section Adaptor
</commit_message>
<xml_diff>
--- a/Users/blieu/Temporary_Work/Section Adaptor Calculations.xlsx
+++ b/Users/blieu/Temporary_Work/Section Adaptor Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19182" windowHeight="6432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Outer Diameter(in)</t>
   </si>
@@ -78,6 +78,39 @@
   </si>
   <si>
     <t>http://www.engineeringtoolbox.com/euler-column-formula-d_1813.html</t>
+  </si>
+  <si>
+    <t>Thermal Stress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulus of Elasticity </t>
+  </si>
+  <si>
+    <t>CTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature Change </t>
+  </si>
+  <si>
+    <t>http://asm.matweb.com/search/SpecificMaterial.asp?bassnum=MA6061t6</t>
+  </si>
+  <si>
+    <t>Deformation thermal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strain </t>
+  </si>
+  <si>
+    <t>dt*E*CTE</t>
+  </si>
+  <si>
+    <t>Stress = E*Strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Thickness Required </t>
+  </si>
+  <si>
+    <t>hoop stress addition</t>
   </si>
 </sst>
 </file>
@@ -430,36 +463,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.26171875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.3671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1">
+        <f>68.9*10^9</f>
+        <v>68900000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <f>14*10^-6</f>
+        <v>1.4E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -467,8 +517,15 @@
         <f>10*10^6</f>
         <v>10000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <f>250-77</f>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -476,35 +533,84 @@
         <f>3.14*(B1^4-B2^4)*(1/64)</f>
         <v>2.8576989746093751</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <f>F1*F2*F3</f>
+        <v>166875800</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <f>F2*B5*F3</f>
+        <v>1.4532E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <f>(3.14)^2*B3*B4*(1/(0.65*B5))^2</f>
-        <v>1157781.4271062864</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18524502.833700582</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <f>F5/B5</f>
+        <v>2.4220000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <f>F6*F1</f>
+        <v>166875800</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9">
+        <f>710*2*F8*(1/(2*F7))</f>
+        <v>1.2763983753186501E-5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -512,7 +618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -520,7 +626,7 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -528,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -536,7 +642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -544,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -552,12 +658,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>